<commit_message>
Updated Registration functionality with mark attendance feature with changes in registration route and registration route, Also added feature to update real time encoding for successful login after registration at the moment. Also handled scenario to stop duplicate face registration.
</commit_message>
<xml_diff>
--- a/app/TestCases/Registration/TestCase_RegistrationPage.xlsx
+++ b/app/TestCases/Registration/TestCase_RegistrationPage.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{642D4C3E-933E-4CE7-81E4-FC34225672F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rehana\Desktop\Big_Data_Semester1\Programming_for_big-data\Project\FacialRecognitionAttendanceSystem\app\TestCases\Registration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7D20BE-06DB-4C27-9098-30CB075A3DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <r>
       <t>Positive Test Cases</t>
@@ -155,6 +160,24 @@
   </si>
   <si>
     <t>The system should allow special characters in the username.</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>Verify duplicate registration with same face</t>
+  </si>
+  <si>
+    <t>1. Enter registration fields</t>
+  </si>
+  <si>
+    <t>2. Click Add user</t>
+  </si>
+  <si>
+    <t>The system should not allow registring same face.(Pass)</t>
+  </si>
+  <si>
+    <t>This can allo same face if camera quality is low, lightening issue(Fail)</t>
   </si>
 </sst>
 </file>
@@ -612,18 +635,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" customWidth="1"/>
     <col min="2" max="2" width="59.5" customWidth="1"/>
-    <col min="3" max="3" width="83.25" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="83.19921875" customWidth="1"/>
+    <col min="4" max="5" width="56.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="22.5" customHeight="1">
@@ -634,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="15.75">
+    <row r="2" spans="1:4" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -648,7 +671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -677,12 +700,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4">
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75"/>
     <row r="10" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1">
       <c r="A10" s="3">
         <v>2</v>
@@ -691,7 +713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="15.75">
+    <row r="11" spans="1:4" s="2" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -705,7 +727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -719,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -733,7 +755,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -747,7 +769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -761,7 +783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -773,6 +795,28 @@
       </c>
       <c r="D16" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Web API for OTP-based email verification system for new user registrations.Also,Added course removal feature with course enrollment.
</commit_message>
<xml_diff>
--- a/app/TestCases/Registration/TestCase_RegistrationPage.xlsx
+++ b/app/TestCases/Registration/TestCase_RegistrationPage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rehana\Desktop\Big_Data_Semester1\Programming_for_big-data\Project\FacialRecognitionAttendanceSystem\app\TestCases\Registration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7D20BE-06DB-4C27-9098-30CB075A3DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E56FE-BE68-4618-94EB-B7A163C85EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <r>
       <t>Positive Test Cases</t>
@@ -178,6 +178,33 @@
   </si>
   <si>
     <t>This can allo same face if camera quality is low, lightening issue(Fail)</t>
+  </si>
+  <si>
+    <t>Enter all required fields for registartion in above test.</t>
+  </si>
+  <si>
+    <t>Click Add new User</t>
+  </si>
+  <si>
+    <t>User should redirect to verify OTP page</t>
+  </si>
+  <si>
+    <t>Enter OTP received</t>
+  </si>
+  <si>
+    <t>An OTP should receive on the  registered email</t>
+  </si>
+  <si>
+    <t>Redirected to registration page</t>
+  </si>
+  <si>
+    <t>Registration should be done successfully</t>
+  </si>
+  <si>
+    <t>verify otp is received during registration and Email after Registration</t>
+  </si>
+  <si>
+    <t>Testing in different machine with dofferent webcam setting can give issue(Fail)</t>
   </si>
 </sst>
 </file>
@@ -635,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -646,7 +673,8 @@
     <col min="1" max="1" width="13.09765625" customWidth="1"/>
     <col min="2" max="2" width="59.5" customWidth="1"/>
     <col min="3" max="3" width="83.19921875" customWidth="1"/>
-    <col min="4" max="5" width="56.59765625" customWidth="1"/>
+    <col min="4" max="4" width="62.8984375" customWidth="1"/>
+    <col min="5" max="5" width="56.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="22.5" customHeight="1">
@@ -705,118 +733,163 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A10" s="3">
+    <row r="8" spans="1:4">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A15" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1">
-      <c r="A11" s="2" t="s">
+    <row r="16" spans="1:4" s="2" customFormat="1">
+      <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="C18" t="s">
+    <row r="23" spans="1:4">
+      <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="D24" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>